<commit_message>
Combinr changes in metadata + textt briefs
-Metadata: create a column code_merge using the name for the variables in the output clean data (some have the name_portal and others have code, so we merge using code_merge)
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{67091234-C320-4288-B14B-B7F991048018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3567C1A0-3193-479A-B312-2BF4336ECA14}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{67091234-C320-4288-B14B-B7F991048018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94B514A0-38AF-4DA6-BE98-1AFDDCF98981}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="166">
   <si>
     <t>name_portal</t>
   </si>
@@ -56,9 +56,6 @@
     <t>vacBCG</t>
   </si>
   <si>
-    <t>vacDTP1</t>
-  </si>
-  <si>
     <t>vacHEPB3</t>
   </si>
   <si>
@@ -233,18 +230,9 @@
     <t>org_learning</t>
   </si>
   <si>
-    <t>inst_births</t>
-  </si>
-  <si>
     <t>educ_exp</t>
   </si>
   <si>
-    <t>minprof_r_prim</t>
-  </si>
-  <si>
-    <t>minprof_m_prim</t>
-  </si>
-  <si>
     <t>out_school</t>
   </si>
   <si>
@@ -257,9 +245,6 @@
     <t>HPV_vac</t>
   </si>
   <si>
-    <t>emp_high_skill</t>
-  </si>
-  <si>
     <t>health_exp</t>
   </si>
   <si>
@@ -434,9 +419,6 @@
     <t>**Youth unemployment (%).** Unemployment among youth ages 15-24 is **`ind_value' percent** (*`ind_year'*)</t>
   </si>
   <si>
-    <t>**Participation rate in organized learning (% of children one year before the official primary entry age).** **`ind_value' percent** of children one year before the official primary entry age (*`ind_year'*) participate in an organized learning program.</t>
-  </si>
-  <si>
     <t>**Youth literacy rate (%).** The literacy rate for youth ages 15-24 years is **`ind_value' percent** (*`ind_year'*)</t>
   </si>
   <si>
@@ -531,6 +513,30 @@
   </si>
   <si>
     <t>**Internally Displaced Persons (%).** The rate of internally displaced persons of concern to UNHCR, as percentage of  population is **`ind_value' persons** (*`ind_year'*)</t>
+  </si>
+  <si>
+    <t>vacDTP3</t>
+  </si>
+  <si>
+    <t>high_skill</t>
+  </si>
+  <si>
+    <t>ECedu</t>
+  </si>
+  <si>
+    <t>insbirths</t>
+  </si>
+  <si>
+    <t>minprof_m_endprim</t>
+  </si>
+  <si>
+    <t>minprof_r_endprim</t>
+  </si>
+  <si>
+    <t>**Participation rate in organized learning (% of children one year before the official primary entry age).** As in (*`ind_year'*) ,  **`ind_value' percent** of children one year before the official primary entry age participate in an organized learning program.</t>
+  </si>
+  <si>
+    <t>**Gross enrolment ratio, early childhood education** The gross enrolment ratein early childhood education is  **`ind_value' ** (*`ind_year'*)</t>
   </si>
 </sst>
 </file>
@@ -901,11 +907,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,418 +927,418 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1340,13 +1346,13 @@
         <v>2</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1354,130 +1360,130 @@
         <v>3</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E33" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1485,316 +1491,316 @@
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E35" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E36" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E37" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E38" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E39" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E40" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E42" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C43" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E44" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E45" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E46" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E47" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E48" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E49" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E50" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E51" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C52" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E52" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E53" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1802,390 +1808,404 @@
         <v>4</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E54" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>158</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C55" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E55" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E56" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C57" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E57" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="C58" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E58" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C59" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E59" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E60" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C61" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E61" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C62" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E62" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C63" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D63" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E63" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C64" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E64" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E65" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C66" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D66" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E66" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>72</v>
+        <v>159</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C67" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E67" s="6"/>
     </row>
     <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C68" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E68" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C69" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D69" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E69" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C70" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E70" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C71" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D71" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E71" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E72" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C73" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C74" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C75" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C76" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D76" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" t="s">
+        <v>96</v>
+      </c>
+      <c r="D77" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>160</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C77" t="s">
-        <v>101</v>
-      </c>
-      <c r="D77" t="s">
-        <v>56</v>
+      <c r="B78" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C78" t="s">
+        <v>96</v>
+      </c>
+      <c r="D78" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Match titles in graphs and texts
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{67091234-C320-4288-B14B-B7F991048018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94B514A0-38AF-4DA6-BE98-1AFDDCF98981}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{67091234-C320-4288-B14B-B7F991048018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4E2B369-D256-4544-B801-BB92A90F995D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,12 +413,6 @@
     <t>**Pre-primary school gross enrollment ratio (%).** The pre-primary school gross enrollment ratio is **`ind_value' percent** (*`ind_year'*)</t>
   </si>
   <si>
-    <t>**Adult unemployment (%).** Unemployment among adults more than 25 years old is **`ind_value' percent** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Youth unemployment (%).** Unemployment among youth ages 15-24 is **`ind_value' percent** (*`ind_year'*)</t>
-  </si>
-  <si>
     <t>**Youth literacy rate (%).** The literacy rate for youth ages 15-24 years is **`ind_value' percent** (*`ind_year'*)</t>
   </si>
   <si>
@@ -537,6 +531,12 @@
   </si>
   <si>
     <t>**Gross enrolment ratio, early childhood education** The gross enrolment ratein early childhood education is  **`ind_value' ** (*`ind_year'*)</t>
+  </si>
+  <si>
+    <t>**Adult unemployment (%).** The unemployment rate among adults more than 25 years old is **`ind_value' percent** (*`ind_year'*)</t>
+  </si>
+  <si>
+    <t>**Youth unemployment (%).** The unemployment rate among youth ages 15-24 is **`ind_value' percent** (*`ind_year'*)</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -576,6 +576,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -623,6 +629,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,8 +920,8 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1056,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C8" t="s">
         <v>96</v>
@@ -1063,7 +1073,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
         <v>96</v>
@@ -1080,7 +1090,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
         <v>96</v>
@@ -1097,7 +1107,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
         <v>96</v>
@@ -1165,7 +1175,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
         <v>96</v>
@@ -1422,7 +1432,7 @@
         <v>51</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C31" t="s">
         <v>96</v>
@@ -1440,7 +1450,7 @@
         <v>26</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C32" t="s">
         <v>96</v>
@@ -1457,7 +1467,7 @@
         <v>39</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C33" t="s">
         <v>96</v>
@@ -1519,7 +1529,7 @@
         <v>53</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C37" t="s">
         <v>96</v>
@@ -1723,7 +1733,7 @@
         <v>11</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="C49" t="s">
         <v>96</v>
@@ -1740,7 +1750,7 @@
         <v>14</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>125</v>
+        <v>165</v>
       </c>
       <c r="C50" t="s">
         <v>96</v>
@@ -1757,7 +1767,7 @@
         <v>43</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C51" t="s">
         <v>96</v>
@@ -1774,7 +1784,7 @@
         <v>44</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C52" t="s">
         <v>96</v>
@@ -1791,7 +1801,7 @@
         <v>45</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C53" t="s">
         <v>96</v>
@@ -1822,7 +1832,7 @@
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>83</v>
@@ -1859,7 +1869,7 @@
         <v>61</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C57" t="s">
         <v>96</v>
@@ -1871,29 +1881,29 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="58" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C58" t="s">
-        <v>96</v>
-      </c>
-      <c r="D58" t="s">
-        <v>55</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="B58" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E58" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C59" t="s">
         <v>96</v>
@@ -1924,10 +1934,10 @@
     </row>
     <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C61" t="s">
         <v>96</v>
@@ -1941,10 +1951,10 @@
     </row>
     <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C62" t="s">
         <v>96</v>
@@ -1978,7 +1988,7 @@
         <v>65</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C64" t="s">
         <v>96</v>
@@ -1995,7 +2005,7 @@
         <v>66</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C65" t="s">
         <v>96</v>
@@ -2012,7 +2022,7 @@
         <v>67</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C66" t="s">
         <v>96</v>
@@ -2026,10 +2036,10 @@
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C67" t="s">
         <v>96</v>
@@ -2044,7 +2054,7 @@
         <v>68</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C68" t="s">
         <v>96</v>
@@ -2061,7 +2071,7 @@
         <v>91</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C69" t="s">
         <v>96</v>
@@ -2126,10 +2136,10 @@
     </row>
     <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C73" t="s">
         <v>96</v>
@@ -2140,10 +2150,10 @@
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C74" t="s">
         <v>96</v>
@@ -2154,10 +2164,10 @@
     </row>
     <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C75" t="s">
         <v>96</v>
@@ -2168,10 +2178,10 @@
     </row>
     <row r="76" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C76" t="s">
         <v>96</v>
@@ -2182,10 +2192,10 @@
     </row>
     <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C77" t="s">
         <v>96</v>
@@ -2196,10 +2206,10 @@
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C78" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Update one variable name
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{67091234-C320-4288-B14B-B7F991048018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E9AA58C-BBED-4235-ACBE-9B90818330D2}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{67091234-C320-4288-B14B-B7F991048018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EE6E6E3-C162-4260-AF3F-CEBD908780C7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>emp_nifl_a</t>
   </si>
   <si>
-    <t>eap_2wap_mf_a</t>
-  </si>
-  <si>
     <t>une_2eap_mf_a</t>
   </si>
   <si>
@@ -537,6 +534,9 @@
   </si>
   <si>
     <t>**Gross enrollment ratio, early childhood education** The gross enrolment ratein early childhood education is  **`ind_value' ** (*`ind_year'*)</t>
+  </si>
+  <si>
+    <t>eap_dwap_mf_a</t>
   </si>
 </sst>
 </file>
@@ -910,8 +910,8 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,152 +927,152 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1080,16 +1080,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1097,16 +1097,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1114,67 +1114,67 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1182,163 +1182,163 @@
         <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1346,13 +1346,13 @@
         <v>2</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1360,130 +1360,130 @@
         <v>3</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1491,316 +1491,316 @@
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1808,33 +1808,33 @@
         <v>4</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1842,370 +1842,370 @@
         <v>5</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C58" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C61" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C66" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D67" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E67" s="6"/>
     </row>
     <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D68" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="C70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C71" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D71" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C72" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D72" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D73" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D74" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C75" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D75" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D76" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D78" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update texts based on comments made by Wendy, Rythia and German
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AC321A-0D31-41A5-BA47-5C3177A24E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BFF1C6-8383-45C9-B913-80F00B7D4DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -248,15 +248,9 @@
     <t>ok</t>
   </si>
   <si>
-    <t>**Stillbirth rate (per 1,000 total births).** The share of babies born with no sign of life at 28 weeks or more of gestation is **`ind_value' per 1,000 total births** (*`ind_year'*)</t>
-  </si>
-  <si>
     <t>persons</t>
   </si>
   <si>
-    <t>**Life expectancy at birth (years).** Life expectancy at birth is **`ind_value' years** (*`ind_year'*)</t>
-  </si>
-  <si>
     <t>HIV_inc_1019</t>
   </si>
   <si>
@@ -269,15 +263,6 @@
     <t>youth_adult_un</t>
   </si>
   <si>
-    <t>**Asylum seekers (persons).** The number of asylum seekers, specifically individuals awaiting a decision on their asylum claims under the mandate of the United Nations High Commissioner for Refugees (UNHCR), is **`ind_value' persons** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Out of school children (per 1,000 children aged 14).** The number of out-of-school children of primary school age is **`ind_value' persons** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Refugees (persons).** The number of refugees, under the mandate of the United Nations High Commissioner for Refugees (UNHCR), is **`ind_value' persons** (*`ind_year'*)</t>
-  </si>
-  <si>
     <t>netenrt_ls</t>
   </si>
   <si>
@@ -311,30 +296,6 @@
     <t>minprof_r_endprim</t>
   </si>
   <si>
-    <t>**HIV incidence rate (per 1,000 uninfected).** The estimated incidence rate, i.e., the number of new HIV infections per 1,000 uninfected adolescents ages 10-19 years, is **`ind_value'** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Adolescent fertility rate (births/1000 women).** The adolescent fertility rate, i.e., the number of births for every 1000 women ages 15-19, is **`ind_value'** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Maternal mortality ratio (per 100,000 live births).** For every 100,000 live births, **`ind_value' women** (*`ind_year'*) die from pregnancy related causes</t>
-  </si>
-  <si>
-    <t>**Youth mortality rate (per 1,000 youth aged 15).**  The mortality rate at ages 15–24 is **`ind_value' per 1,000 youth aged 15** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Child mortality rate (per 1,000 youth aged 5).**  The mortality rate at ages 5–14 is **`ind_value' per 1,000 children aged 15** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Adolescent suicide rates (per 100,000 population).** The suicide rate among youth aged 15-19 years is **`ind_value' per 100,000 population** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Youth to adult unemployment ratio (%).** The ratio of youth to adult unemployment is **`ind_value'** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Neonatal mortality rate (per 1,000 live births).** The neonatal mortality rate is **`ind_value' per 1,000 live births** (*`ind_year'*)</t>
-  </si>
-  <si>
     <t>emp_2wap_f_a</t>
   </si>
   <si>
@@ -578,199 +539,238 @@
     <t>**Gross enrollment ratio, early childhood education</t>
   </si>
   <si>
-    <t>**Health care facilities with basic hygiene services (%).** The share of health care facilities with functional hand hygiene facilities near toilets is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Schools with basic hygiene services (%).** The share of schools with handwashing facilities with water and soap available is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Health care facilities with basic sanitation services (%).** The share of health care facilities with improved sanitation facilities is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Schools with basic sanitation services (%).** The share of schools with improved sanitation facilities is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Health care facilities with basic water services  (%).** The share of health care facilities with water available from an improved source is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Children engaged in child labor (%).** The share of children aged 5-17 years who are engaged in economic activities is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Care seeking for children with diarrhoea (%).** The share of children (ages 0-5) with diarrhea who attended a health facility is  **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Prevalence of hypertension (%).** The prevalence of hypertension among people ages 30-79 is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Prevalence of insufficient physical activity (%).** The share of school-going adolescents ages 11-17 years not meeting WHO recommendations on physical activity for health is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Completeness of birth registration (%).** Complete birth registration is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Gross school enrollment rate, secondary (%).** The secondary school gross enrollment rate is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Gross school enrollment rate, tertiary (%).** The tertiary school gross enrollment rate is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Minimum meal frequency (%).** Adequate meal frequency among children 0-23 months is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Probability of dying from NCDs (%).** The probability of dying from non-communicable diseases between the ages of 30 to 70 is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Care seeking for children with pneumonia symptoms (%).** The share of children with less than five years with pneumonia symptoms who were taken to an appropriate health provider is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Primary school completion rate (%).** Primary school completion rate is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Lower secondary school completion rate (%).** Lower secondary school completion rate is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Upper secondary school completion rate (%).** Upper secondary school completion rate is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Gross enrollment, early childhood education (%). The gross enrollment ratio in early childhood educational development programs is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Pre-primary school gross enrollment ratio (%).** The pre-primary school gross enrollment ratio is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Qualified teachers in primary education (%).** The share of qualified teachers in primary education is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Qualified teachers in secondary education (%).** The proportion of qualified teachers in secondary education is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Primary schools with access to electricity (%).** The share of primary schools with access to electricity is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Adult unemployment rate (%).** The unemployment rate among adults more than 25 years old is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Youth unemployment rate (%).** The unemployment rate among youth ages 15-24 is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Youth literacy rate (%).** The literacy rate for youth ages 15-24 years is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Diphtheria vaccination, third dose (%).** The percentage of surviving infants who received the third dose of diphtheria vaccine is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Current education expenditure (% GDP).** The current education expenditure as a percentage of GDP is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Satisfied demand for family planning (% of women).** The percentage of women ages 15-49 years who had their need for family planning satisfied is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**HPV vaccination, last dose (%).** The percentage of females who received the last dose of HPV vaccine is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Current health expenditure (%).** The current health expenditure as a percentage of GDP is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Female labor force participation rate (%).** The female labor force participation rate (ages +25) as a percentage of the working population is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Male labor force participation rate (%).** The male labor force participation rate (ages +25) as a percentage of the working population is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Adult informal employment rate (%).** The percentage of adults ages +25 engaged in informal employment is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Youth informal employment rate (%).** The percentage of youth ages 15-24 involved in informal employment is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Prevalence of obesity among adults (%).** The percentage of adults aged 18+ years with obesity (BMI ≥ 30) is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Over-age primary students (%).** The percentage of over-age primary students, i.e., students who are older than the typical age for their respective school level, is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Over-age lower secondary students (%).** The percentage of over-age lower secondary students, i.e., students who are older than the typical age for their respective school level, is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**BCG vaccination (%).** The percentage of live births who received the BCG vaccine against tuberculosis is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Hepatitis B vaccination, third dose (%).** The percentage of surviving infants who received the hepatitis B vaccine is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Refugees (%).** The rate of refugees, under the mandate of the United Nations High Commissioner for Refugees (UNHCR), as a percentage of the population is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Asylum seekers (%).** The rate of asylum seekers, specifically individuals awaiting a decision on their asylum claims under the mandate of the United Nations High Commissioner for Refugees (UNHCR), as a percentage of the population is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Internally Displaced Persons (%).** The rate of internally displaced persons of concern to UNHCR, as a percentage of the population is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Net school enrollment rate, lower secondary.** The percentage of school net enrolment at lower secondary is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Out of school children (%).** The percentage of primary-school-age children who are out of school is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**ITN use by children.** The percentage of children (under age 5) who slept under an insecticide-treated mosquito net the night prior to being surveyed is **`ind_value'%** (*`ind_year'*)</t>
-  </si>
-  <si>
-    <t>**Exclusive breastfeeding (%).** In *`ind_year'*, **`ind_value'%** of infants 0-5 months were fed exclusively with breast milk</t>
-  </si>
-  <si>
-    <t>**Postnatal care for newborns (%).** In *`ind_year'*, **`ind_value'%** of newborns have postnatal contact with health providers during their first two days of life</t>
-  </si>
-  <si>
-    <t>**Care seeking for febrile children (%).** In *`ind_year'*, **`ind_value'%** of children under age 5 with fever sought treatment or advice</t>
-  </si>
-  <si>
-    <t>**Postnatal care for mothers (%).** In *`ind_year'*, **`ind_value'%** of mothers (aged 15-49) have postnatal contact with health providers during their first two days of life</t>
-  </si>
-  <si>
-    <t>**Youth not in employment, education or training (%).** In *`ind_year'*, **`ind_value'%** of the youth ages 15-24 are not in employment, education or training</t>
-  </si>
-  <si>
-    <t>**Repetition rate in primary education (%).** In *`ind_year'*, **`ind_value'%** of students in primary education remained in the same grade in the following school year</t>
-  </si>
-  <si>
-    <t>**Learning poverty (%).** In *`ind_year'*, **`ind_value'%** of 10-year-olds cannot read and understand a simple text by the end of primary school</t>
-  </si>
-  <si>
-    <t>**Prevalence of sexual violence (%).** In *`ind_year'*, **`ind_value'%** of women aged 18-29 years experienced sexual violence by age 18</t>
-  </si>
-  <si>
-    <t>**Prevalence of anaemia in children (%).** In *`ind_year'*, **`ind_value'%** of children aged 6–59 months has anaemia</t>
-  </si>
-  <si>
-    <t>**Population with basic handwashing facility (%)**. In *`ind_year'*, **`ind_value'%** of population has access to a handwashing facility with soap and water at home</t>
-  </si>
-  <si>
-    <t>**Population with basic sanitation services (%)**. In *`ind_year'*, **`ind_value'%** of population has access to an improved sanitation facility at home</t>
-  </si>
-  <si>
-    <t>**Population with basic drinking water services (%)**. In *`ind_year'*, **`ind_value'%** of population (*`ind_year'*) has access to an improved drinking water source, where collection time is not more than 30 minutes</t>
-  </si>
-  <si>
-    <t>**Children who are developmentally on track (%).** In *`ind_year'*, **`ind_value'%** of children 24-59 months are developmentally on track in health, learning and psychosocial well-being</t>
-  </si>
-  <si>
-    <t>**Participation rate in organized learning (%).** In *`ind_year'*, **`ind_value'%** of children one year before the official primary entry age participate in an organized learning program</t>
-  </si>
-  <si>
-    <t>**Institutional births (%).** In *`ind_year'*, **`ind_value'% of births** occurred in health facilities</t>
-  </si>
-  <si>
-    <t>**Minimum proficiency in reading, primary (%).** In *`ind_year'*, **`ind_value'% of children** achieved the minimum learning outcomes in reading at the end of primary school</t>
-  </si>
-  <si>
-    <t>**Minimum proficiency in mathematics, primary (%).** In *`ind_year'*, **`ind_value'% of children** achieved the minimum learning outcomes in mathematics at the end of primary school</t>
-  </si>
-  <si>
-    <t>**High skill employment rate (%).** In *`ind_year'*, **`ind_value'%** of total employed adults are high-skilled (levels 3-4)</t>
-  </si>
-  <si>
-    <t>**Gross enrollment ratio, early childhood education.** The gross enrolment rate in early childhood education is **`ind_value'% ** (*`ind_year'*)</t>
+    <t>**Health care facilities with basic hygiene services (%).** The share of health care facilities with functional hand hygiene facilities near toilets is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Schools with basic hygiene services (%).** The share of schools with handwashing facilities with water and soap available is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Health care facilities with basic sanitation services (%).** The share of health care facilities with improved sanitation facilities is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Schools with basic sanitation services (%).** The share of schools with improved sanitation facilities is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Health care facilities with basic water services  (%).** The share of health care facilities with water available from an improved source is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Exclusive breastfeeding (%).** In `ind_year', **`ind_value'%** of infants 0-5 months were fed exclusively with breast milk</t>
+  </si>
+  <si>
+    <t>**Postnatal care for newborns (%).** In `ind_year', **`ind_value'%** of newborns have postnatal contact with health providers during their first two days of life</t>
+  </si>
+  <si>
+    <t>**Care seeking for febrile children (%).** In `ind_year', **`ind_value'%** of children under age 5 with fever sought treatment or advice</t>
+  </si>
+  <si>
+    <t>**Postnatal care for mothers (%).** In `ind_year', **`ind_value'%** of mothers (aged 15-49) have postnatal contact with health providers during their first two days of life</t>
+  </si>
+  <si>
+    <t>**Children engaged in child labor (%).** The share of children aged 5-17 years who are engaged in economic activities is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Care seeking for children with diarrhoea (%).** The share of children (ages 0-5) with diarrhea who attended a health facility is  **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Youth not in employment, education or training (%).** In `ind_year', **`ind_value'%** of the youth ages 15-24 are not in employment, education or training</t>
+  </si>
+  <si>
+    <t>**Youth informal employment rate (%).** The percentage of youth ages 15-24 involved in informal employment is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Prevalence of hypertension (%).** The prevalence of hypertension among people ages 30-79 is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Prevalence of insufficient physical activity (%).** The share of school-going adolescents ages 11-17 years not meeting WHO recommendations on physical activity for health is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Adolescent fertility rate (births/1000 women).** The adolescent fertility rate, i.e., the number of births for every 1000 women ages 15-19, is **`ind_value'** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Completeness of birth registration (%).** Complete birth registration is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Gross school enrollment rate, secondary (%).** The secondary school gross enrollment rate is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Gross school enrollment rate, tertiary (%).** The tertiary school gross enrollment rate is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Minimum meal frequency (%).** Adequate meal frequency among children 0-23 months is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Prevalence of obesity among adults (%).** The percentage of adults aged 18+ years with obesity (BMI ≥ 30) is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Probability of dying from NCDs (%).** The probability of dying from non-communicable diseases between the ages of 30 to 70 is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Repetition rate in primary education (%).** In `ind_year', **`ind_value'%** of students in primary education remained in the same grade in the following school year</t>
+  </si>
+  <si>
+    <t>**Learning poverty (%).** In `ind_year', **`ind_value'%** of 10-year-olds cannot read and understand a simple text by the end of primary school</t>
+  </si>
+  <si>
+    <t>**Prevalence of sexual violence (%).** In `ind_year', **`ind_value'%** of women aged 18-29 years experienced sexual violence by age 18</t>
+  </si>
+  <si>
+    <t>**Prevalence of anaemia in children (%).** In `ind_year', **`ind_value'%** of children aged 6–59 months has anaemia</t>
+  </si>
+  <si>
+    <t>**Care seeking for children with pneumonia symptoms (%).** The share of children with less than five years with pneumonia symptoms who were taken to an appropriate health provider is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Primary school completion rate (%).** Primary school completion rate is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Lower secondary school completion rate (%).** Lower secondary school completion rate is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Upper secondary school completion rate (%).** Upper secondary school completion rate is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Gross enrollment, early childhood education (%). The gross enrollment ratio in early childhood educational development programs is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Pre-primary school gross enrollment ratio (%).** The pre-primary school gross enrollment ratio is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Over-age primary students (%).** The percentage of over-age primary students, i.e., students who are older than the typical age for their respective school level, is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Over-age lower secondary students (%).** The percentage of over-age lower secondary students, i.e., students who are older than the typical age for their respective school level, is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Qualified teachers in primary education (%).** The share of qualified teachers in primary education is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Qualified teachers in secondary education (%).** The proportion of qualified teachers in secondary education is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Primary schools with access to electricity (%).** The share of primary schools with access to electricity is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Youth unemployment rate (%).** The unemployment rate among youth ages 15-24 is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Population with basic handwashing facility (%)**. In `ind_year', **`ind_value'%** of population has access to a handwashing facility with soap and water at home</t>
+  </si>
+  <si>
+    <t>**Population with basic sanitation services (%)**. In `ind_year', **`ind_value'%** of population has access to an improved sanitation facility at home</t>
+  </si>
+  <si>
+    <t>**Population with basic drinking water services (%)**. In `ind_year', **`ind_value'%** of population (`ind_year') has access to an improved drinking water source, where collection time is not more than 30 minutes</t>
+  </si>
+  <si>
+    <t>**BCG vaccination (%).** The percentage of live births who received the BCG vaccine against tuberculosis is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Diphtheria vaccination, third dose (%).** The percentage of surviving infants who received the third dose of diphtheria vaccine is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Hepatitis B vaccination, third dose (%).** The percentage of surviving infants who received the hepatitis B vaccine is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Children who are developmentally on track (%).** In `ind_year', **`ind_value'%** of children 24-59 months are developmentally on track in health, learning and psychosocial well-being</t>
+  </si>
+  <si>
+    <t>**Participation rate in organized learning (%).** In `ind_year', **`ind_value'%** of children one year before the official primary entry age participate in an organized learning program</t>
+  </si>
+  <si>
+    <t>**Current education expenditure (% GDP).** The current education expenditure as a percentage of GDP is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Youth literacy rate (%).** The literacy rate for youth ages 15-24 years is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Satisfied demand for family planning (% of women).** The percentage of women ages 15-49 years who had their need for family planning satisfied is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**HPV vaccination, last dose (%).** The percentage of females who received the last dose of HPV vaccine is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**High skill employment rate (%).** In `ind_year', **`ind_value'%** of total employed adults are high-skilled (levels 3-4)</t>
+  </si>
+  <si>
+    <t>**Current health expenditure (%).** The current health expenditure as a percentage of GDP is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**HIV incidence rate (per 1,000 uninfected).** The estimated incidence rate, i.e., the number of new HIV infections per 1,000 uninfected adolescents ages 10-19 years, is **`ind_value'** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**ITN use by children.** The percentage of children (under age 5) who slept under an insecticide-treated mosquito net the night prior to being surveyed is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Youth to adult unemployment ratio (%).** The ratio of youth to adult unemployment is **`ind_value'** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Net school enrollment rate, lower secondary.** The percentage of school net enrolment at lower secondary is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Out of school children (%).** The percentage of primary-school-age children who are out of school is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Refugees (%).** The rate of refugees, under the mandate of the United Nations High Commissioner for Refugees (UNHCR), as a percentage of the population is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Asylum seekers (%).** The rate of asylum seekers, specifically individuals awaiting a decision on their asylum claims under the mandate of the United Nations High Commissioner for Refugees (UNHCR), as a percentage of the population is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Internally Displaced Persons (%).** The rate of internally displaced persons of concern to UNHCR, as a percentage of the population is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Gross enrollment ratio, early childhood education.** The gross enrolment rate in early childhood education is **`ind_value'% ** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Asylum seekers (persons).** The number of asylum seekers, specifically individuals awaiting a decision on their asylum claims under the mandate of the United Nations High Commissioner for Refugees (UNHCR), is **`ind_value'** persons (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Maternal mortality ratio (per 100,000 live births).** For every 100,000 live births, **`ind_value'** women (`ind_year') die from pregnancy related causes</t>
+  </si>
+  <si>
+    <t>**Youth mortality rate (per 1,000 youth aged 15).**  The mortality rate at ages 15–24 is **`ind_value'** per 1,000 youth aged 15 (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Child mortality rate (per 1,000 youth aged 5).**  The mortality rate at ages 5–14 is **`ind_value'** per 1,000 children aged 15 (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Neonatal mortality rate (per 1,000 live births).** The neonatal mortality rate is **`ind_value'** per 1,000 live births (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Life expectancy at birth (years).** Life expectancy at birth is **`ind_value'** years (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Stillbirth rate (per 1,000 total births).** The share of babies born with no sign of life at 28 weeks or more of gestation is **`ind_value'** per 1,000 total births (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Adolescent suicide rates (per 100,000 population).** The suicide rate among youth aged 15-19 years is **`ind_value'** per 100,000 population (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Institutional births (%).** In `ind_year', **`ind_value'%** of births occurred in health facilities</t>
+  </si>
+  <si>
+    <t>**Minimum proficiency in reading, primary (%).** In `ind_year', **`ind_value'%** of children achieved the minimum learning outcomes in reading at the end of primary school</t>
+  </si>
+  <si>
+    <t>**Minimum proficiency in mathematics, primary (%).** In `ind_year', **`ind_value'%** of children achieved the minimum learning outcomes in mathematics at the end of primary school</t>
+  </si>
+  <si>
+    <t>**Out of school children (per 1,000 children aged 14).** The number of out-of-school children of primary school age is **`ind_value'** persons (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Refugees (persons).** The number of refugees, under the mandate of the United Nations High Commissioner for Refugees (UNHCR), is **`ind_value'** persons (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Female labor force participation rate (%).** The female labor force participation rate (ages 25+) as a percentage of the working population is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Male labor force participation rate (%).** The male labor force participation rate (ages 25+) as a percentage of the working population is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Adult informal employment rate (%).** The percentage of adults ages 25+ engaged in informal employment is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Adult unemployment rate (%).** The unemployment rate among adults older than 25 years old is **`ind_value'%** (`ind_year')</t>
   </si>
 </sst>
 </file>
@@ -1140,8 +1140,8 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1169,7 @@
         <v>67</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1177,16 +1177,16 @@
         <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>76</v>
+        <v>227</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1194,7 +1194,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C34" si="0">IF(D3="%","%","")</f>
@@ -1207,7 +1207,7 @@
         <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1215,7 +1215,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -1228,7 +1228,7 @@
         <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1236,7 +1236,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -1249,7 +1249,7 @@
         <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -1270,7 +1270,7 @@
         <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1278,7 +1278,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -1291,7 +1291,7 @@
         <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1299,7 +1299,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>225</v>
+        <v>171</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -1312,7 +1312,7 @@
         <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1320,7 +1320,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>226</v>
+        <v>172</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -1333,7 +1333,7 @@
         <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>227</v>
+        <v>173</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -1354,7 +1354,7 @@
         <v>68</v>
       </c>
       <c r="F10" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1362,7 +1362,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>228</v>
+        <v>174</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -1375,7 +1375,7 @@
         <v>68</v>
       </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -1396,7 +1396,7 @@
         <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1404,7 +1404,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -1417,15 +1417,15 @@
         <v>68</v>
       </c>
       <c r="F13" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -1438,15 +1438,15 @@
         <v>68</v>
       </c>
       <c r="F14" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>211</v>
+        <v>241</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -1459,7 +1459,7 @@
         <v>68</v>
       </c>
       <c r="F15" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1467,7 +1467,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>229</v>
+        <v>177</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -1480,7 +1480,7 @@
         <v>68</v>
       </c>
       <c r="F16" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1488,7 +1488,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>212</v>
+        <v>242</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -1501,7 +1501,7 @@
         <v>68</v>
       </c>
       <c r="F17" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1509,7 +1509,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -1522,7 +1522,7 @@
         <v>68</v>
       </c>
       <c r="F18" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1530,7 +1530,7 @@
         <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -1543,7 +1543,7 @@
         <v>68</v>
       </c>
       <c r="F19" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1551,7 +1551,7 @@
         <v>48</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -1564,7 +1564,7 @@
         <v>68</v>
       </c>
       <c r="F20" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1572,7 +1572,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>91</v>
+        <v>181</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -1582,7 +1582,7 @@
         <v>68</v>
       </c>
       <c r="F21" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1590,7 +1590,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -1603,7 +1603,7 @@
         <v>68</v>
       </c>
       <c r="F22" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1611,7 +1611,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>92</v>
+        <v>228</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -1621,7 +1621,7 @@
         <v>68</v>
       </c>
       <c r="F23" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1629,7 +1629,7 @@
         <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -1642,7 +1642,7 @@
         <v>68</v>
       </c>
       <c r="F24" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1650,7 +1650,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -1663,7 +1663,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1671,7 +1671,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -1684,7 +1684,7 @@
         <v>68</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1692,7 +1692,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>93</v>
+        <v>229</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -1702,7 +1702,7 @@
         <v>68</v>
       </c>
       <c r="F27" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1710,7 +1710,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>94</v>
+        <v>230</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -1720,7 +1720,7 @@
         <v>68</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1728,7 +1728,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>97</v>
+        <v>231</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -1738,7 +1738,7 @@
         <v>68</v>
       </c>
       <c r="F29" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1746,7 +1746,7 @@
         <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -1759,7 +1759,7 @@
         <v>68</v>
       </c>
       <c r="F30" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1767,7 +1767,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -1780,7 +1780,7 @@
         <v>68</v>
       </c>
       <c r="F31" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1788,7 +1788,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -1801,7 +1801,7 @@
         <v>68</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1809,7 +1809,7 @@
         <v>25</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>231</v>
+        <v>189</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -1822,7 +1822,7 @@
         <v>68</v>
       </c>
       <c r="F33" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1830,7 +1830,7 @@
         <v>38</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -1843,7 +1843,7 @@
         <v>68</v>
       </c>
       <c r="F34" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1851,7 +1851,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>71</v>
+        <v>232</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" ref="C35:C66" si="1">IF(D35="%","%","")</f>
@@ -1864,7 +1864,7 @@
         <v>68</v>
       </c>
       <c r="F35" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1872,7 +1872,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>69</v>
+        <v>233</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
@@ -1882,7 +1882,7 @@
         <v>68</v>
       </c>
       <c r="F36" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1890,7 +1890,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>95</v>
+        <v>234</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
@@ -1900,7 +1900,7 @@
         <v>68</v>
       </c>
       <c r="F37" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1908,7 +1908,7 @@
         <v>52</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>233</v>
+        <v>191</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
@@ -1921,7 +1921,7 @@
         <v>68</v>
       </c>
       <c r="F38" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1929,7 +1929,7 @@
         <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
@@ -1942,7 +1942,7 @@
         <v>68</v>
       </c>
       <c r="F39" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1950,7 +1950,7 @@
         <v>33</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
@@ -1963,7 +1963,7 @@
         <v>68</v>
       </c>
       <c r="F40" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1971,7 +1971,7 @@
         <v>30</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
@@ -1984,7 +1984,7 @@
         <v>68</v>
       </c>
       <c r="F41" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1992,7 +1992,7 @@
         <v>14</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
@@ -2005,7 +2005,7 @@
         <v>68</v>
       </c>
       <c r="F42" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2013,7 +2013,7 @@
         <v>15</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
@@ -2026,7 +2026,7 @@
         <v>68</v>
       </c>
       <c r="F43" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2034,7 +2034,7 @@
         <v>34</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
@@ -2047,7 +2047,7 @@
         <v>68</v>
       </c>
       <c r="F44" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2055,7 +2055,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
@@ -2068,7 +2068,7 @@
         <v>68</v>
       </c>
       <c r="F45" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2076,7 +2076,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
@@ -2089,7 +2089,7 @@
         <v>68</v>
       </c>
       <c r="F46" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
         <v>19</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
@@ -2110,7 +2110,7 @@
         <v>68</v>
       </c>
       <c r="F47" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -2118,7 +2118,7 @@
         <v>20</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
@@ -2131,7 +2131,7 @@
         <v>68</v>
       </c>
       <c r="F48" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2139,7 +2139,7 @@
         <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
@@ -2152,7 +2152,7 @@
         <v>68</v>
       </c>
       <c r="F49" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2160,7 +2160,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>202</v>
+        <v>243</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
@@ -2173,7 +2173,7 @@
         <v>68</v>
       </c>
       <c r="F50" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2194,7 +2194,7 @@
         <v>68</v>
       </c>
       <c r="F51" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2202,7 +2202,7 @@
         <v>42</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
@@ -2215,7 +2215,7 @@
         <v>68</v>
       </c>
       <c r="F52" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2223,7 +2223,7 @@
         <v>43</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
@@ -2236,7 +2236,7 @@
         <v>68</v>
       </c>
       <c r="F53" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v>44</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
@@ -2257,7 +2257,7 @@
         <v>68</v>
       </c>
       <c r="F54" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2265,7 +2265,7 @@
         <v>4</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
@@ -2278,15 +2278,15 @@
         <v>68</v>
       </c>
       <c r="F55" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
@@ -2299,7 +2299,7 @@
         <v>68</v>
       </c>
       <c r="F56" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>5</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
@@ -2320,7 +2320,7 @@
         <v>68</v>
       </c>
       <c r="F57" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2328,7 +2328,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="1"/>
@@ -2341,7 +2341,7 @@
         <v>68</v>
       </c>
       <c r="F58" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2349,7 +2349,7 @@
         <v>60</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>238</v>
+        <v>211</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
@@ -2362,15 +2362,15 @@
         <v>68</v>
       </c>
       <c r="F59" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
@@ -2383,7 +2383,7 @@
         <v>68</v>
       </c>
       <c r="F60" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2391,7 +2391,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
@@ -2404,15 +2404,15 @@
         <v>68</v>
       </c>
       <c r="F61" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
@@ -2425,15 +2425,15 @@
         <v>68</v>
       </c>
       <c r="F62" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
@@ -2446,7 +2446,7 @@
         <v>68</v>
       </c>
       <c r="F63" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2454,20 +2454,20 @@
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>77</v>
+        <v>238</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E64" t="s">
         <v>68</v>
       </c>
       <c r="F64" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2475,7 +2475,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
@@ -2488,7 +2488,7 @@
         <v>68</v>
       </c>
       <c r="F65" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2496,7 +2496,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="1"/>
@@ -2509,7 +2509,7 @@
         <v>68</v>
       </c>
       <c r="F66" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C79" si="2">IF(D67="%","%","")</f>
@@ -2530,15 +2530,15 @@
         <v>68</v>
       </c>
       <c r="F67" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="2"/>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="E68" s="6"/>
       <c r="F68" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2557,7 +2557,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="2"/>
@@ -2570,15 +2570,15 @@
         <v>68</v>
       </c>
       <c r="F69" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>90</v>
+        <v>218</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="2"/>
@@ -2591,15 +2591,15 @@
         <v>68</v>
       </c>
       <c r="F70" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="2"/>
@@ -2612,36 +2612,36 @@
         <v>68</v>
       </c>
       <c r="F71" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>78</v>
+        <v>239</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E72" t="s">
         <v>68</v>
       </c>
       <c r="F72" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>96</v>
+        <v>220</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="2"/>
@@ -2654,15 +2654,15 @@
         <v>68</v>
       </c>
       <c r="F73" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="2"/>
@@ -2672,15 +2672,15 @@
         <v>54</v>
       </c>
       <c r="F74" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="2"/>
@@ -2690,15 +2690,15 @@
         <v>54</v>
       </c>
       <c r="F75" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="2"/>
@@ -2708,15 +2708,15 @@
         <v>54</v>
       </c>
       <c r="F76" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="2"/>
@@ -2726,15 +2726,15 @@
         <v>54</v>
       </c>
       <c r="F77" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="2"/>
@@ -2744,15 +2744,15 @@
         <v>54</v>
       </c>
       <c r="F78" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="2"/>
@@ -2762,7 +2762,7 @@
         <v>54</v>
       </c>
       <c r="F79" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New graph format and fix texts issues
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887E8426-D11E-49FA-B8F3-71AA5A60C469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{887E8426-D11E-49FA-B8F3-71AA5A60C469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF3BDA8B-DE2F-4680-8F9B-9BC3D0ACDCBD}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -557,24 +557,15 @@
     <t>**Exclusive breastfeeding (%).** In `ind_year', **`ind_value'%** of infants 0-5 months were fed exclusively with breast milk</t>
   </si>
   <si>
-    <t>**Postnatal care for newborns (%).** In `ind_year', **`ind_value'%** of newborns have postnatal contact with health providers during their first two days of life</t>
-  </si>
-  <si>
     <t>**Care seeking for febrile children (%).** In `ind_year', **`ind_value'%** of children under age 5 with fever sought treatment or advice</t>
   </si>
   <si>
-    <t>**Postnatal care for mothers (%).** In `ind_year', **`ind_value'%** of mothers (aged 15-49) have postnatal contact with health providers during their first two days of life</t>
-  </si>
-  <si>
     <t>**Children engaged in child labor (%).** The share of children aged 5-17 years who are engaged in economic activities is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
     <t>**Care seeking for children with diarrhoea (%).** The share of children (ages 0-5) with diarrhea who attended a health facility is  **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Youth not in employment, education or training (%).** In `ind_year', **`ind_value'%** of the youth ages 15-24 are not in employment, education or training</t>
-  </si>
-  <si>
     <t>**Youth informal employment rate (%).** The percentage of youth ages 15-24 involved in informal employment is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -608,15 +599,9 @@
     <t>**Repetition rate in primary education (%).** In `ind_year', **`ind_value'%** of students in primary education remained in the same grade in the following school year</t>
   </si>
   <si>
-    <t>**Learning poverty (%).** In `ind_year', **`ind_value'%** of 10-year-olds cannot read and understand a simple text by the end of primary school</t>
-  </si>
-  <si>
     <t>**Prevalence of sexual violence (%).** In `ind_year', **`ind_value'%** of women aged 18-29 years experienced sexual violence by age 18</t>
   </si>
   <si>
-    <t>**Prevalence of anaemia in children (%).** In `ind_year', **`ind_value'%** of children aged 6–59 months has anaemia</t>
-  </si>
-  <si>
     <t>**Care seeking for children with pneumonia symptoms (%).** The share of children with less than five years with pneumonia symptoms who were taken to an appropriate health provider is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -653,15 +638,6 @@
     <t>**Youth unemployment rate (%).** The unemployment rate among youth ages 15-24 is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Population with basic handwashing facility (%)**. In `ind_year', **`ind_value'%** of population has access to a handwashing facility with soap and water at home</t>
-  </si>
-  <si>
-    <t>**Population with basic sanitation services (%)**. In `ind_year', **`ind_value'%** of population has access to an improved sanitation facility at home</t>
-  </si>
-  <si>
-    <t>**Population with basic drinking water services (%)**. In `ind_year', **`ind_value'%** of population (`ind_year') has access to an improved drinking water source, where collection time is not more than 30 minutes</t>
-  </si>
-  <si>
     <t>**BCG vaccination (%).** The percentage of live births who received the BCG vaccine against tuberculosis is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -671,12 +647,6 @@
     <t>**Hepatitis B vaccination, third dose (%).** The percentage of surviving infants who received the hepatitis B vaccine is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Children who are developmentally on track (%).** In `ind_year', **`ind_value'%** of children 24-59 months are developmentally on track in health, learning and psychosocial well-being</t>
-  </si>
-  <si>
-    <t>**Participation rate in organized learning (%).** In `ind_year', **`ind_value'%** of children one year before the official primary entry age participate in an organized learning program</t>
-  </si>
-  <si>
     <t>**Current education expenditure (% GDP).** The current education expenditure as a percentage of GDP is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -689,9 +659,6 @@
     <t>**HPV vaccination, last dose (%).** The percentage of females who received the last dose of HPV vaccine is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**High skill employment rate (%).** In `ind_year', **`ind_value'%** of total employed adults are high-skilled (levels 3-4)</t>
-  </si>
-  <si>
     <t>**Current health expenditure (%).** The current health expenditure as a percentage of GDP is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -771,6 +738,39 @@
   </si>
   <si>
     <t>**Child mortality rate (per 1,000 children aged 5).**  The mortality rate for children at ages 5-14 is **`ind_value'** per 1,000 children aged 5 (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Participation rate in organized learning (%).** In `ind_year', **`ind_value'%** of children one year before the official primary entry age participated in an organized learning program</t>
+  </si>
+  <si>
+    <t>**High skill employment rate (%).** In `ind_year', **`ind_value'%** of total employed adults were high-skilled (levels 3-4)</t>
+  </si>
+  <si>
+    <t>**Postnatal care for newborns (%).** In `ind_year', **`ind_value'%** of newborns had postnatal contact with health providers during their first two days of life</t>
+  </si>
+  <si>
+    <t>**Postnatal care for mothers (%).** In `ind_year', **`ind_value'%** of mothers (aged 15-49) had postnatal contact with health providers during their first two days of life</t>
+  </si>
+  <si>
+    <t>**Youth not in employment, education or training (%).** In `ind_year', **`ind_value'%** of the youth ages 15-24 were not in employment, education or training</t>
+  </si>
+  <si>
+    <t>**Learning poverty (%).** In `ind_year', **`ind_value'%** of 10-year-olds could not read and understand a simple text by the end of primary school</t>
+  </si>
+  <si>
+    <t>**Prevalence of anaemia in children (%).** In `ind_year', **`ind_value'%** of children aged 6–59 months had anaemia</t>
+  </si>
+  <si>
+    <t>**Population with basic handwashing facility (%)**. In `ind_year', **`ind_value'%** of population had access to a handwashing facility with soap and water at home</t>
+  </si>
+  <si>
+    <t>**Population with basic sanitation services (%)**. In `ind_year', **`ind_value'%** of population had access to an improved sanitation facility at home</t>
+  </si>
+  <si>
+    <t>**Population with basic drinking water services (%)**. In `ind_year', **`ind_value'%** of population (`ind_year') had access to an improved drinking water source, where collection time is not more than 30 minutes</t>
+  </si>
+  <si>
+    <t>**Children who are developmentally on track (%).** In `ind_year', **`ind_value'%** of children 24-59 months were developmentally on track in health, learning and psychosocial well-being</t>
   </si>
 </sst>
 </file>
@@ -1140,8 +1140,8 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1177,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="D2" t="s">
         <v>69</v>
@@ -1320,7 +1320,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>172</v>
+        <v>235</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -1341,7 +1341,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -1362,7 +1362,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>174</v>
+        <v>236</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -1383,7 +1383,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -1404,7 +1404,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -1425,7 +1425,7 @@
         <v>85</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -1446,7 +1446,7 @@
         <v>86</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -1467,7 +1467,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -1488,7 +1488,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -1509,7 +1509,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -1530,7 +1530,7 @@
         <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -1551,7 +1551,7 @@
         <v>48</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -1572,7 +1572,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -1590,7 +1590,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -1611,7 +1611,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -1629,7 +1629,7 @@
         <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -1650,7 +1650,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -1671,7 +1671,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -1692,7 +1692,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -1710,7 +1710,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -1728,7 +1728,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -1746,7 +1746,7 @@
         <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -1767,7 +1767,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -1788,7 +1788,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -1809,7 +1809,7 @@
         <v>25</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>189</v>
+        <v>238</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -1830,7 +1830,7 @@
         <v>38</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -1851,7 +1851,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" ref="C35:C66" si="1">IF(D35="%","%","")</f>
@@ -1872,7 +1872,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
@@ -1890,7 +1890,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
@@ -1908,7 +1908,7 @@
         <v>52</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>191</v>
+        <v>239</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
@@ -1929,7 +1929,7 @@
         <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
@@ -1950,7 +1950,7 @@
         <v>33</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
@@ -1971,7 +1971,7 @@
         <v>30</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
@@ -1992,7 +1992,7 @@
         <v>14</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
@@ -2013,7 +2013,7 @@
         <v>15</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
@@ -2034,7 +2034,7 @@
         <v>34</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
@@ -2055,7 +2055,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
@@ -2076,7 +2076,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
@@ -2097,7 +2097,7 @@
         <v>19</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
@@ -2118,7 +2118,7 @@
         <v>20</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
@@ -2139,7 +2139,7 @@
         <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
@@ -2160,7 +2160,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
@@ -2181,7 +2181,7 @@
         <v>13</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
@@ -2202,7 +2202,7 @@
         <v>42</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>204</v>
+        <v>240</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
@@ -2223,7 +2223,7 @@
         <v>43</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>205</v>
+        <v>241</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
@@ -2244,7 +2244,7 @@
         <v>44</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>206</v>
+        <v>242</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
@@ -2265,7 +2265,7 @@
         <v>4</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
@@ -2286,7 +2286,7 @@
         <v>79</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
@@ -2307,7 +2307,7 @@
         <v>5</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
@@ -2328,7 +2328,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>210</v>
+        <v>243</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="1"/>
@@ -2349,7 +2349,7 @@
         <v>60</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
@@ -2370,7 +2370,7 @@
         <v>82</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
@@ -2391,7 +2391,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
@@ -2412,7 +2412,7 @@
         <v>84</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
@@ -2433,7 +2433,7 @@
         <v>83</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
@@ -2454,7 +2454,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
@@ -2475,7 +2475,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
@@ -2496,7 +2496,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="1"/>
@@ -2517,7 +2517,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C79" si="2">IF(D67="%","%","")</f>
@@ -2538,7 +2538,7 @@
         <v>80</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="2"/>
@@ -2557,7 +2557,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="2"/>
@@ -2578,7 +2578,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="2"/>
@@ -2599,7 +2599,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="2"/>
@@ -2620,7 +2620,7 @@
         <v>72</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="2"/>
@@ -2641,7 +2641,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="2"/>
@@ -2662,7 +2662,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="2"/>
@@ -2680,7 +2680,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="2"/>
@@ -2698,7 +2698,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="2"/>
@@ -2716,7 +2716,7 @@
         <v>77</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="2"/>
@@ -2734,7 +2734,7 @@
         <v>78</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="2"/>
@@ -2752,7 +2752,7 @@
         <v>81</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Cambios a pedido de Wendy
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFFE4B9-CD5A-4227-B246-8CB0FB37D612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{8BFFE4B9-CD5A-4227-B246-8CB0FB37D612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FB4F277-DBA4-4F66-8A30-3FDA094D49EF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -314,9 +314,6 @@
     <t>**Postnatal care for newborns.** In `ind_year', **`ind_value'%** of newborns had postnatal contact with health providers during their first two days of life</t>
   </si>
   <si>
-    <t>**Care seeking for febrile children.** In `ind_year', **`ind_value'%** of children under age 5 with fever sought treatment or advice</t>
-  </si>
-  <si>
     <t>**Care seeking for children with diarrhoea.** The share of children (ages 0-5) with diarrhea who attended a health facility is  **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -326,63 +323,27 @@
     <t>**Maternal mortality ratio.** For every 100,000 live births, **`ind_value'** women (`ind_year') die from pregnancy related causes</t>
   </si>
   <si>
-    <t>**Gross school enrollment rate, tertiary.** The tertiary school gross enrollment rate is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
     <t>**Neonatal mortality rate.** The neonatal mortality rate is **`ind_value'** per 1,000 live births (`ind_year')</t>
   </si>
   <si>
     <t>**Probability of dying from NCDs.** The probability of dying from non-communicable diseases between the ages of 30 to 70 is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Repetition rate in primary education.** In `ind_year', **`ind_value'%** of students in primary education remained in the same grade in the following school year</t>
-  </si>
-  <si>
-    <t>**Learning poverty.** In `ind_year', **`ind_value'%** of 10-year-olds could not read and understand a simple text by the end of primary school</t>
-  </si>
-  <si>
     <t>**Life expectancy at birth.** Life expectancy at birth is **`ind_value'** years (`ind_year')</t>
   </si>
   <si>
     <t>**Stillbirth rate.** The share of babies born with no sign of life at 28 weeks or more of gestation is **`ind_value'** per 1,000 total births (`ind_year')</t>
   </si>
   <si>
-    <t>**Care seeking for children with pneumonia symptoms.** The share of children with less than five years with pneumonia symptoms who were taken to an appropriate health provider is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
     <t>**Pre-primary school gross enrollment ratio.** The pre-primary school gross enrollment ratio is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Qualified teachers in primary education.** The share of qualified teachers in primary education is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Primary schools with access to electricity.** The share of primary schools with access to electricity is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Adult unemployment rate.** The unemployment rate among adults older than 25 years old is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Youth unemployment rate.** The unemployment rate among youth ages 15-24 is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Population with basic handwashing facility.** In `ind_year', **`ind_value'%** of population had access to a handwashing facility with soap and water at home</t>
-  </si>
-  <si>
-    <t>**Population with basic sanitation services.** In `ind_year', **`ind_value'%** of population had access to an improved sanitation facility at home</t>
-  </si>
-  <si>
     <t>**Institutional births.** In `ind_year', **`ind_value'%** of births occurred in health facilities</t>
   </si>
   <si>
     <t>**Current education expenditure.** The current education expenditure as a percentage of GDP is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Minimum proficiency in reading, primary.** In `ind_year', **`ind_value'%** of children achieved the minimum learning outcomes in reading at the end of primary school</t>
-  </si>
-  <si>
-    <t>**Minimum proficiency in mathematics, primary.** In `ind_year', **`ind_value'%** of children achieved the minimum learning outcomes in mathematics at the end of primary school</t>
-  </si>
-  <si>
     <t>**High skill employment rate.** In `ind_year', **`ind_value'%** of total employed adults were high-skilled (levels 3-4)</t>
   </si>
   <si>
@@ -392,9 +353,6 @@
     <t>**Refugees.** The number of refugees, under the mandate of the United Nations High Commissioner for Refugees (UNHCR), is **`ind_value'** persons (`ind_year')</t>
   </si>
   <si>
-    <t>**Youth to adult unemployment ratio.** The ratio of youth to adult unemployment is **`ind_value'** (`ind_year')</t>
-  </si>
-  <si>
     <t>**Refugees.** The rate of refugees, under the mandate of the United Nations High Commissioner for Refugees (UNHCR), as a percentage of the population is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -413,36 +371,21 @@
     <t>**Exclusive breastfeeding.** In `ind_year', **`ind_value'%** of infants ages 0-5 months were fed exclusively with breast milk</t>
   </si>
   <si>
-    <t>**Postnatal care for mothers.** In `ind_year', **`ind_value'%** of mothers (ages 15-49) had postnatal contact with health providers during their first two days of life</t>
-  </si>
-  <si>
     <t>**Children engaged in child labor.** The share of children (ages 5-17) who are engaged in economic activities is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
     <t>**Prevalence of insufficient physical activity.** The share of school-going adolescents (ages 11-17) not meeting WHO recommendations on physical activity for health is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Over-age lower secondary students.** The percentage of lower secondary students who are older than the typical age for their respective school level is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
     <t>**Children who are developmentally on track.** In `ind_year', **`ind_value'%** of children (ages 24-59 months) were developmentally on track in health, learning and psychosocial well-being</t>
   </si>
   <si>
-    <t>**Youth literacy rate.** The literacy rate for youth (ages 15-24) is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
     <t>**HIV incidence rate.** The estimated number of new HIV infections per 1,000 uninfected adolescents (ages 10-19 years) is **`ind_value'** (`ind_year')</t>
   </si>
   <si>
-    <t>**Qualified teachers in secondary education.** The share of qualified teachers in secondary education is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
     <t>**BCG vaccination rate.** In `ind_year', **`ind_value'%** of infants received the BCG vaccine against tuberculosis</t>
   </si>
   <si>
-    <t>**Diphtheria vaccination rate, third dose.** In `ind_year', **`ind_value'%** of infants received the third dose of diphtheria vaccine</t>
-  </si>
-  <si>
     <t>**Hepatitis B vaccination rate, third dose.** In `ind_year', **`ind_value'%** of infants received the hepatitis B vaccine</t>
   </si>
   <si>
@@ -455,88 +398,145 @@
     <t xml:space="preserve">**Gross school enrollment rate, secondary.** In `ind_year', **`ind_value'%** of children of secondary school-age were enrolled at that level </t>
   </si>
   <si>
-    <t>**Satisfied demand for family planning.** In `ind_year', **`ind_value'%** of women (ages 15-49) had their need for family planning satisfied</t>
-  </si>
-  <si>
     <t>**Out of school children.** In `ind_year', **`ind_value'%** of primary-school-age children were out of school</t>
   </si>
   <si>
     <t>**Gross enrollment rate, early childhood education.** In `ind_year', **`ind_value'%** of children were enrolled at early childhood education</t>
   </si>
   <si>
-    <t>**Prevalence of anaemia in children.** In `ind_year', **`ind_value'%** of children at ages 6–59 months had anaemia</t>
-  </si>
-  <si>
     <t>**Out of school children.** The number of out-of-school children of primary school age is **`ind_value'** per 1,000 children at age 14 (`ind_year')</t>
   </si>
   <si>
     <t>**Health care facilities with basic hygiene services.** The share of health care facilities with hygiene facilities near toilets is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Female labor force participation rate.** Female labor force participation (ages 25+) as a percentage of the working population is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Male labor force participation rate.** Male labor force participation (ages 25+) as a percentage of the working population is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Upper secondary school completion rate.** The upper secondary school completion rate is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Lower secondary school completion rate.** The lower secondary school completion rate is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Primary school completion rate.** The primary school completion rate is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
     <t>**Youth not in employment, education or training.** In `ind_year', **`ind_value'%** of youth (ages 15-24) were not in employment, education or training</t>
   </si>
   <si>
     <t>**Asylum seekers (persons).** The number of individuals awaiting a decision on their asylum claims under the mandate of the United Nations High Commissioner for Refugees (UNHCR) is **`ind_value'** persons (`ind_year')</t>
   </si>
   <si>
-    <t>**Adult informal employment rate.** The rate of informal employment among adults (ages 25+) is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Youth informal employment rate.** The rate of informal employment youths (ages 15-24) is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Completeness of birth registration.** Complete birth registration rate is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Over-age primary students.** The percentage of primary students who are older than the typical age for their respective school level is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Population with basic drinking water services.** In `ind_year', **`ind_value'%** of population had access to an improved drinking water source, where collection time is not more than 30 minutes</t>
-  </si>
-  <si>
     <t>**Net school enrollment rate, lower secondary.** The percentage of lower secondary school-aged children enrolled at lower secondary is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Participation rate in organized learning.** In `ind_year', **`ind_value'%** of children participated in an organized learning program in the year before the official primary school entry age</t>
-  </si>
-  <si>
     <t>**Adolescent fertility rate.** The number of births for every 1,000 women ages 15-19 is **`ind_value'** (`ind_year')</t>
   </si>
   <si>
-    <t>**Minimum meal frequency.** Adequate meal frequency among children ages 0-23 months is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Prevalence of sexual violence.** In `ind_year', **`ind_value'%** of women ages 18-29 years experienced sexual violence by the age of 18</t>
-  </si>
-  <si>
     <t>**Gross enrollment in early childhood education.** In `ind_year',  **`ind_value'%**  of children were enrolled at early childhood education</t>
   </si>
   <si>
-    <t>**Prevalence of obesity among adults.** The percentage of adults ages 18+ years with obesity (BMI ≥ 30) is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Adolescent suicide rates.** The suicide rate among youth ages 15-19 years is **`ind_value'** per 100,000 population (`ind_year')</t>
-  </si>
-  <si>
     <t>**Child mortality rate.**  The mortality rate for children ages 5-14 is **`ind_value'** per 1,000 children aged 5 (`ind_year')</t>
   </si>
   <si>
     <t>**Youth mortality rate.**  The mortality rate of youth ages 15–24 is **`ind_value'** per 1,000 youth aged 15 (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Care seeking for febrile children.** In `ind_year', **`ind_value'%** of children under age 5 with a fever sought treatment or advice</t>
+  </si>
+  <si>
+    <t>**Postnatal care for mothers.** In `ind_year', **`ind_value'%** of mothers (ages 15-49) had postnatal contact with health providers within 2 days of giving birth</t>
+  </si>
+  <si>
+    <t>**Female labor force participation rate.** Female labor force participation as a percentage of the female working-age population (ages 25+) is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Male labor force participation rate.** Male labor force participation as a percentage of the male working-age population (ages 25+)  is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Adult informal employment rate.** The rate of informal employment among working adults (ages 25+) is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Youth informal employment rate.** The rate of informal employment among working youth (ages 15-24) is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Completeness of birth registration.** Complete birth registration as a share of children under age 5 is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Gross school enrollment rate, tertiary.** Tertiary school enrollment as a percentage of people ages is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Minimum meal frequency.** The percentage of children ages 6-23 months who consume solid, semi-solid or soft foods at least the minimum number of times during the day is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Prevalence of obesity among adults.** The percentage of adults ages 18+ years who are obese is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Repetition rate in primary education.** In `ind_year', **`ind_value'%** of students in primary school remained in the same grade in the following school year</t>
+  </si>
+  <si>
+    <t>**Learning poverty.** In `ind_year', **`ind_value'%** of children at the end-of-primary age could not read and understand a simple text, adjusted by out-of-school children</t>
+  </si>
+  <si>
+    <t>**Prevalence of sexual violence.** In `ind_year', **`ind_value'%** of women ages 18-29 experienced sexual violence by the age of 18</t>
+  </si>
+  <si>
+    <t>**Adolescent suicide rates.** The suicide rate among youth ages 15-19 years is **`ind_value'** per 100,000 youth (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Prevalence of anemia in children.** In `ind_year', **`ind_value'%** of children at ages 6–59 months had anemia</t>
+  </si>
+  <si>
+    <t>**Care seeking for children with pneumonia symptoms.** The share of children under age 5 with pneumonia symptoms who were taken to a health provider is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Primary school completion rate.** The proportion of children at the entrance age of the last grade of primary school that are enrolled at that grade (regardless of age) is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Lower secondary school completion rate.** The proportion of children at the entrance age of the last grade of lower secondary school that are enrolled at that grade (regardless of age) is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Upper secondary school completion rate.** The proportion of children or youth aged 3-5 years above the intended age for the last grade of upper secondary school who have completed that grade is **`ind_value'%** (`ind_year') </t>
+  </si>
+  <si>
+    <t>**Over-age primary students.** The percentage of primary school students who are older than the typical age for their respective school level is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Over-age lower secondary students.** The percentage of lower secondary school students who are older than the typical age for their respective school level is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Qualified teachers in primary education.** The share of  teachers in primary education who have at least the minimum academic qualifications required for teaching is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Qualified teachers in secondary education.** The share of teachers in secondary education who have at least the minimum academic qualifications required for teaching is is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Primary school electricity access.** The share of primary schools with access to electricity is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Adult unemployment rate.** Unemployed adults as a share of the adult labor force (ages +25) is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Youth unemployment rate.** Unemployed youth as a share of the youth labor force (ages 15-24) is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Population with basic handwashing facility.** In `ind_year', **`ind_value'%** of the population had access to a handwashing facility with soap and water at home</t>
+  </si>
+  <si>
+    <t>**Population with basic sanitation services.** In `ind_year', **`ind_value'%** of the population had access to improved sanitation facilities at home</t>
+  </si>
+  <si>
+    <t>**Population with basic drinking water services.** In `ind_year', **`ind_value'%** of the population had access to an improved drinking water source within 30 minutes of their home</t>
+  </si>
+  <si>
+    <t>**Diphtheria vaccination rate, third dose.** In `ind_year', **`ind_value'%** of infants received the third dose of the diphtheria vaccine</t>
+  </si>
+  <si>
+    <t>**Participation rate in organized learning.** In `ind_year', **`ind_value'%** of children who were one year younger than the official primary school entry age participated in an organized learning program</t>
+  </si>
+  <si>
+    <t>**Minimum proficiency in reading, primary.** In `ind_year', **`ind_value'%** of children who completed primary school achieved the minimum learning outcomes in reading</t>
+  </si>
+  <si>
+    <t>**Minimum proficiency in mathematics, primary.** In `ind_year', **`ind_value'%** of children who completed primary school  achieved the minimum learning outcomes in mathematics</t>
+  </si>
+  <si>
+    <t>**Youth literacy rate.** The share of youth (ages 15-24) who are literate is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Satisfied demand for family planning.** In `ind_year', **`ind_value'%** of women (ages 15-49) who wanted family planning services received them</t>
+  </si>
+  <si>
+    <t>**Youth to adult unemployment ratio.** The ratio of the youth unemployment rate to the adult unemployment rate is **`ind_value'** (`ind_year')</t>
   </si>
 </sst>
 </file>
@@ -575,7 +575,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -619,10 +619,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,20 +910,20 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="68.33203125" customWidth="1"/>
-    <col min="7" max="7" width="33.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="68.28515625" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -939,12 +943,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
         <v>69</v>
@@ -957,12 +961,12 @@
         <v xml:space="preserve">**Asylum seekers (persons).** </v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C34" si="0">IF(D3="%","%","")</f>
@@ -979,7 +983,7 @@
         <v xml:space="preserve">**Health care facilities with basic hygiene services.** </v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1001,12 +1005,12 @@
         <v xml:space="preserve">**Schools with basic hygiene services.** </v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -1023,12 +1027,12 @@
         <v xml:space="preserve">**Health care facilities with basic sanitation services.** </v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -1045,7 +1049,7 @@
         <v xml:space="preserve">**Schools with basic sanitation services.** </v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1067,12 +1071,12 @@
         <v xml:space="preserve">**Health care facilities with basic water services.** </v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -1089,7 +1093,7 @@
         <v xml:space="preserve">**Exclusive breastfeeding.** </v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1111,12 +1115,12 @@
         <v xml:space="preserve">**Postnatal care for newborns.** </v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -1133,12 +1137,12 @@
         <v xml:space="preserve">**Care seeking for febrile children.** </v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -1155,12 +1159,12 @@
         <v xml:space="preserve">**Postnatal care for mothers.** </v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -1177,12 +1181,12 @@
         <v xml:space="preserve">**Children engaged in child labor.** </v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -1199,12 +1203,12 @@
         <v xml:space="preserve">**Care seeking for children with diarrhoea.** </v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>85</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -1221,12 +1225,12 @@
         <v xml:space="preserve">**Female labor force participation rate.** </v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>86</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -1243,12 +1247,12 @@
         <v xml:space="preserve">**Male labor force participation rate.** </v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -1265,12 +1269,12 @@
         <v xml:space="preserve">**Youth not in employment, education or training.** </v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -1287,12 +1291,12 @@
         <v xml:space="preserve">**Adult informal employment rate.** </v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -1309,12 +1313,12 @@
         <v xml:space="preserve">**Youth informal employment rate.** </v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -1331,12 +1335,12 @@
         <v xml:space="preserve">**Prevalence of hypertension.** </v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -1353,12 +1357,12 @@
         <v xml:space="preserve">**Prevalence of insufficient physical activity.** </v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -1372,12 +1376,12 @@
         <v xml:space="preserve">**Adolescent fertility rate.** </v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -1394,12 +1398,12 @@
         <v xml:space="preserve">**Completeness of birth registration.** </v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -1413,12 +1417,12 @@
         <v xml:space="preserve">**Maternal mortality ratio.** </v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -1435,12 +1439,12 @@
         <v xml:space="preserve">**Gross school enrollment rate, secondary.** </v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -1457,34 +1461,34 @@
         <v xml:space="preserve">**Gross school enrollment rate, tertiary.** </v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v>%</v>
-      </c>
-      <c r="D26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" t="str">
+      <c r="B26" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="7" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Minimum meal frequency.** </v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -1498,12 +1502,12 @@
         <v xml:space="preserve">**Youth mortality rate.** </v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -1517,12 +1521,12 @@
         <v xml:space="preserve">**Child mortality rate.** </v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -1536,12 +1540,12 @@
         <v xml:space="preserve">**Neonatal mortality rate.** </v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -1558,12 +1562,12 @@
         <v xml:space="preserve">**Prevalence of obesity among adults.** </v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -1580,12 +1584,12 @@
         <v xml:space="preserve">**Probability of dying from NCDs.** </v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>98</v>
+        <v>140</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -1602,34 +1606,34 @@
         <v xml:space="preserve">**Repetition rate in primary education.** </v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="33" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" t="str">
-        <f t="shared" si="0"/>
-        <v>%</v>
-      </c>
-      <c r="D33" t="s">
-        <v>54</v>
-      </c>
-      <c r="E33" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" t="str">
+      <c r="B33" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="7" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Learning poverty.** </v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -1646,12 +1650,12 @@
         <v xml:space="preserve">**Prevalence of sexual violence.** </v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" ref="C35:C66" si="2">IF(D35="%","%","")</f>
@@ -1668,12 +1672,12 @@
         <v xml:space="preserve">**Life expectancy at birth.** </v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="2"/>
@@ -1687,12 +1691,12 @@
         <v xml:space="preserve">**Stillbirth rate.** </v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="2"/>
@@ -1706,12 +1710,12 @@
         <v xml:space="preserve">**Adolescent suicide rates.** </v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="2"/>
@@ -1725,15 +1729,15 @@
       </c>
       <c r="F38" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">**Prevalence of anaemia in children.** </v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">**Prevalence of anemia in children.** </v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="2"/>
@@ -1750,78 +1754,78 @@
         <v xml:space="preserve">**Care seeking for children with pneumonia symptoms.** </v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C40" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">**Primary school completion rate.** </v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">**Lower secondary school completion rate.** </v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="C40" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D40" t="s">
-        <v>54</v>
-      </c>
-      <c r="E40" t="s">
-        <v>68</v>
-      </c>
-      <c r="F40" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">**Primary school completion rate.** </v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>30</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C41" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D41" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" t="s">
-        <v>68</v>
-      </c>
-      <c r="F41" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">**Lower secondary school completion rate.** </v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C42" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D42" t="s">
-        <v>54</v>
-      </c>
-      <c r="E42" t="s">
-        <v>68</v>
-      </c>
-      <c r="F42" t="str">
+      <c r="C42" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F42" s="7" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Upper secondary school completion rate.** </v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>15</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="2"/>
@@ -1838,12 +1842,12 @@
         <v xml:space="preserve">**Gross enrollment in early childhood education.** </v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>34</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="2"/>
@@ -1860,12 +1864,12 @@
         <v xml:space="preserve">**Pre-primary school gross enrollment ratio.** </v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>17</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="2"/>
@@ -1882,12 +1886,12 @@
         <v xml:space="preserve">**Over-age primary students.** </v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="2"/>
@@ -1904,56 +1908,56 @@
         <v xml:space="preserve">**Over-age lower secondary students.** </v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="47" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C47" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D47" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" t="s">
-        <v>68</v>
-      </c>
-      <c r="F47" t="str">
+      <c r="B47" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="7" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Qualified teachers in primary education.** </v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="48" spans="1:6" s="7" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D48" t="s">
-        <v>54</v>
-      </c>
-      <c r="E48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F48" t="str">
+      <c r="B48" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F48" s="7" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Qualified teachers in secondary education.** </v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="2"/>
@@ -1967,15 +1971,15 @@
       </c>
       <c r="F49" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">**Primary schools with access to electricity.** </v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">**Primary school electricity access.** </v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="2"/>
@@ -1992,12 +1996,12 @@
         <v xml:space="preserve">**Adult unemployment rate.** </v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>13</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="2"/>
@@ -2014,12 +2018,12 @@
         <v xml:space="preserve">**Youth unemployment rate.** </v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>42</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>108</v>
+        <v>156</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="2"/>
@@ -2036,12 +2040,12 @@
         <v xml:space="preserve">**Population with basic handwashing facility.** </v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>43</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="2"/>
@@ -2058,12 +2062,12 @@
         <v xml:space="preserve">**Population with basic sanitation services.** </v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>44</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="2"/>
@@ -2080,12 +2084,12 @@
         <v xml:space="preserve">**Population with basic drinking water services.** </v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>4</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="2"/>
@@ -2102,12 +2106,12 @@
         <v xml:space="preserve">**BCG vaccination rate.** </v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>79</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="2"/>
@@ -2124,12 +2128,12 @@
         <v xml:space="preserve">**Diphtheria vaccination rate, third dose.** </v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>5</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="2"/>
@@ -2146,12 +2150,12 @@
         <v xml:space="preserve">**Hepatitis B vaccination rate, third dose.** </v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="2"/>
@@ -2168,12 +2172,12 @@
         <v xml:space="preserve">**Children who are developmentally on track.** </v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="2"/>
@@ -2190,12 +2194,12 @@
         <v xml:space="preserve">**Participation rate in organized learning.** </v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>82</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="2"/>
@@ -2212,12 +2216,12 @@
         <v xml:space="preserve">**Institutional births.** </v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="2"/>
@@ -2234,12 +2238,12 @@
         <v xml:space="preserve">**Current education expenditure.** </v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>84</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>112</v>
+        <v>161</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="2"/>
@@ -2256,12 +2260,12 @@
         <v xml:space="preserve">**Minimum proficiency in reading, primary.** </v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>83</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="2"/>
@@ -2278,12 +2282,12 @@
         <v xml:space="preserve">**Minimum proficiency in mathematics, primary.** </v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="2"/>
@@ -2300,12 +2304,12 @@
         <v xml:space="preserve">**Out of school children.** </v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="2"/>
@@ -2322,34 +2326,34 @@
         <v xml:space="preserve">**Youth literacy rate.** </v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="66" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C66" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D66" t="s">
-        <v>54</v>
-      </c>
-      <c r="E66" t="s">
-        <v>68</v>
-      </c>
-      <c r="F66" t="str">
+      <c r="B66" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F66" s="7" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Satisfied demand for family planning.** </v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C79" si="3">IF(D67="%","%","")</f>
@@ -2366,32 +2370,31 @@
         <v xml:space="preserve">**HPV vaccination rate, last dose.** </v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="6" t="s">
+    <row r="68" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C68" t="str">
+      <c r="B68" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C68" s="5" t="str">
         <f t="shared" si="3"/>
         <v>%</v>
       </c>
-      <c r="D68" t="s">
-        <v>54</v>
-      </c>
-      <c r="E68" s="6"/>
-      <c r="F68" t="str">
+      <c r="D68" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F68" s="5" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">**High skill employment rate.** </v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>66</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="3"/>
@@ -2408,12 +2411,12 @@
         <v xml:space="preserve">**Current health expenditure.** </v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="3"/>
@@ -2430,12 +2433,12 @@
         <v xml:space="preserve">**HIV incidence rate.** </v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="3"/>
@@ -2452,12 +2455,12 @@
         <v xml:space="preserve">**ITN use by children.** </v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="3"/>
@@ -2474,12 +2477,12 @@
         <v xml:space="preserve">**Refugees.** </v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="3"/>
@@ -2496,12 +2499,12 @@
         <v xml:space="preserve">**Youth to adult unemployment ratio.** </v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="3"/>
@@ -2515,12 +2518,12 @@
         <v xml:space="preserve">**Net school enrollment rate, lower secondary.** </v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="3"/>
@@ -2534,12 +2537,12 @@
         <v xml:space="preserve">**Out of school children.** </v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="3"/>
@@ -2553,12 +2556,12 @@
         <v xml:space="preserve">**Refugees.** </v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="3"/>
@@ -2572,12 +2575,12 @@
         <v xml:space="preserve">**Asylum seekers.** </v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="3"/>
@@ -2591,12 +2594,12 @@
         <v xml:space="preserve">**Internally Displaced Persons.** </v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>81</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Correccion de textos + minor graph bugs
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{8BFFE4B9-CD5A-4227-B246-8CB0FB37D612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FB4F277-DBA4-4F66-8A30-3FDA094D49EF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78280841-B553-44DD-AA52-B8C385311BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -305,12 +305,6 @@
     <t>no_data_start_text</t>
   </si>
   <si>
-    <t>**Schools with basic hygiene services.** The share of schools with handwashing facilities with water and soap available is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Health care facilities with basic water services.** The share of health care facilities with water available from an improved source is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
     <t>**Postnatal care for newborns.** In `ind_year', **`ind_value'%** of newborns had postnatal contact with health providers during their first two days of life</t>
   </si>
   <si>
@@ -344,9 +338,6 @@
     <t>**Current education expenditure.** The current education expenditure as a percentage of GDP is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**High skill employment rate.** In `ind_year', **`ind_value'%** of total employed adults were high-skilled (levels 3-4)</t>
-  </si>
-  <si>
     <t>**Current health expenditure.** The current health expenditure as a percentage of GDP is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -401,9 +392,6 @@
     <t>**Out of school children.** In `ind_year', **`ind_value'%** of primary-school-age children were out of school</t>
   </si>
   <si>
-    <t>**Gross enrollment rate, early childhood education.** In `ind_year', **`ind_value'%** of children were enrolled at early childhood education</t>
-  </si>
-  <si>
     <t>**Out of school children.** The number of out-of-school children of primary school age is **`ind_value'** per 1,000 children at age 14 (`ind_year')</t>
   </si>
   <si>
@@ -416,9 +404,6 @@
     <t>**Asylum seekers (persons).** The number of individuals awaiting a decision on their asylum claims under the mandate of the United Nations High Commissioner for Refugees (UNHCR) is **`ind_value'** persons (`ind_year')</t>
   </si>
   <si>
-    <t>**Net school enrollment rate, lower secondary.** The percentage of lower secondary school-aged children enrolled at lower secondary is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
     <t>**Adolescent fertility rate.** The number of births for every 1,000 women ages 15-19 is **`ind_value'** (`ind_year')</t>
   </si>
   <si>
@@ -431,9 +416,6 @@
     <t>**Youth mortality rate.**  The mortality rate of youth ages 15–24 is **`ind_value'** per 1,000 youth aged 15 (`ind_year')</t>
   </si>
   <si>
-    <t>**Care seeking for febrile children.** In `ind_year', **`ind_value'%** of children under age 5 with a fever sought treatment or advice</t>
-  </si>
-  <si>
     <t>**Postnatal care for mothers.** In `ind_year', **`ind_value'%** of mothers (ages 15-49) had postnatal contact with health providers within 2 days of giving birth</t>
   </si>
   <si>
@@ -449,15 +431,6 @@
     <t>**Youth informal employment rate.** The rate of informal employment among working youth (ages 15-24) is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Completeness of birth registration.** Complete birth registration as a share of children under age 5 is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Gross school enrollment rate, tertiary.** Tertiary school enrollment as a percentage of people ages is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Minimum meal frequency.** The percentage of children ages 6-23 months who consume solid, semi-solid or soft foods at least the minimum number of times during the day is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
     <t>**Prevalence of obesity among adults.** The percentage of adults ages 18+ years who are obese is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -479,27 +452,12 @@
     <t>**Care seeking for children with pneumonia symptoms.** The share of children under age 5 with pneumonia symptoms who were taken to a health provider is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Primary school completion rate.** The proportion of children at the entrance age of the last grade of primary school that are enrolled at that grade (regardless of age) is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Lower secondary school completion rate.** The proportion of children at the entrance age of the last grade of lower secondary school that are enrolled at that grade (regardless of age) is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Upper secondary school completion rate.** The proportion of children or youth aged 3-5 years above the intended age for the last grade of upper secondary school who have completed that grade is **`ind_value'%** (`ind_year') </t>
-  </si>
-  <si>
     <t>**Over-age primary students.** The percentage of primary school students who are older than the typical age for their respective school level is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
     <t>**Over-age lower secondary students.** The percentage of lower secondary school students who are older than the typical age for their respective school level is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Qualified teachers in primary education.** The share of  teachers in primary education who have at least the minimum academic qualifications required for teaching is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
-    <t>**Qualified teachers in secondary education.** The share of teachers in secondary education who have at least the minimum academic qualifications required for teaching is is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
     <t>**Primary school electricity access.** The share of primary schools with access to electricity is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -527,9 +485,6 @@
     <t>**Minimum proficiency in reading, primary.** In `ind_year', **`ind_value'%** of children who completed primary school achieved the minimum learning outcomes in reading</t>
   </si>
   <si>
-    <t>**Minimum proficiency in mathematics, primary.** In `ind_year', **`ind_value'%** of children who completed primary school  achieved the minimum learning outcomes in mathematics</t>
-  </si>
-  <si>
     <t>**Youth literacy rate.** The share of youth (ages 15-24) who are literate is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -537,6 +492,51 @@
   </si>
   <si>
     <t>**Youth to adult unemployment ratio.** The ratio of the youth unemployment rate to the adult unemployment rate is **`ind_value'** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Care seeking for febrile children.** In `ind_year', **`ind_value'%** of children under age 5 with a fever for whom medical advice or treatment was sought</t>
+  </si>
+  <si>
+    <t>**Minimum meal frequency.** The share of children ages 0-23 months who regularly consume an age-appropriate meal is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**High skill employment rate.** In `ind_year', **`ind_value'%** of employed adults worked in high-skilled occupations</t>
+  </si>
+  <si>
+    <t>**Net school enrollment rate, lower secondary.** The percentage of lower secondary school-aged children enrolled at that level is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Upper secondary school completion rate.** Upper secondary school completion rate is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Primary school completion rate.** Primary school completion rate is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Lower secondary school completion rate.** Lower secondary school completion rate is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Qualified teachers in primary education.** The share of primary school teachers who are qualified is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Qualified teachers in secondary education.** The share of secondary school teachers who are qualified is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Schools with basic hygiene services.** The share of schools with handwashing facilities with water and soap is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Health care facilities with basic water services.** The share of health care facilities with water from an improved source is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Completeness of birth registration.** Complete birth registration as a share of total births in `ind_year' is **`ind_value'%**</t>
+  </si>
+  <si>
+    <t>**Gross school enrollment rate, tertiary.** Tertiary school enrollment as a percentage of people ages 18-24 is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Minimum proficiency in mathematics, primary.** In `ind_year', **`ind_value'%** of children who completed primary school achieved the minimum learning outcomes in mathematics</t>
+  </si>
+  <si>
+    <t>**Gross enrollment rate, early childhood education.** In `ind_year', **`ind_value'%** of children were enrolled in a pre-primary school education program</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -617,10 +617,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -910,8 +906,8 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +944,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
         <v>69</v>
@@ -966,7 +962,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C34" si="0">IF(D3="%","%","")</f>
@@ -983,12 +979,12 @@
         <v xml:space="preserve">**Health care facilities with basic hygiene services.** </v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>88</v>
+        <v>160</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -1010,7 +1006,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -1032,7 +1028,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -1054,7 +1050,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>89</v>
+        <v>161</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -1076,7 +1072,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -1098,7 +1094,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -1115,12 +1111,12 @@
         <v xml:space="preserve">**Postnatal care for newborns.** </v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -1142,7 +1138,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -1164,7 +1160,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -1186,7 +1182,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -1208,7 +1204,7 @@
         <v>85</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -1230,7 +1226,7 @@
         <v>86</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -1252,7 +1248,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -1274,7 +1270,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -1296,7 +1292,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -1318,7 +1314,7 @@
         <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -1340,7 +1336,7 @@
         <v>48</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -1362,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -1381,7 +1377,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -1403,7 +1399,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -1422,7 +1418,7 @@
         <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -1444,7 +1440,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -1461,24 +1457,24 @@
         <v xml:space="preserve">**Gross school enrollment rate, tertiary.** </v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C26" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>%</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="7" t="str">
+      <c r="B26" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="5" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Minimum meal frequency.** </v>
       </c>
@@ -1488,7 +1484,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -1507,7 +1503,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -1526,7 +1522,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -1545,7 +1541,7 @@
         <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -1567,7 +1563,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -1589,7 +1585,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -1606,24 +1602,24 @@
         <v xml:space="preserve">**Repetition rate in primary education.** </v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C33" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>%</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="7" t="str">
+      <c r="B33" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="5" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Learning poverty.** </v>
       </c>
@@ -1633,7 +1629,7 @@
         <v>38</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -1655,7 +1651,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" ref="C35:C66" si="2">IF(D35="%","%","")</f>
@@ -1677,7 +1673,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="2"/>
@@ -1696,7 +1692,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="2"/>
@@ -1715,7 +1711,7 @@
         <v>52</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="2"/>
@@ -1737,7 +1733,7 @@
         <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="2"/>
@@ -1754,68 +1750,68 @@
         <v xml:space="preserve">**Care seeking for children with pneumonia symptoms.** </v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C40" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F40" s="7" t="str">
+      <c r="B40" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="5" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Primary school completion rate.** </v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+    <row r="41" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C41" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F41" s="7" t="str">
+      <c r="B41" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" s="5" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Lower secondary school completion rate.** </v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+    <row r="42" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C42" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F42" s="7" t="str">
+      <c r="B42" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F42" s="5" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Upper secondary school completion rate.** </v>
       </c>
@@ -1825,7 +1821,7 @@
         <v>15</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="2"/>
@@ -1847,7 +1843,7 @@
         <v>34</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="2"/>
@@ -1869,7 +1865,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="2"/>
@@ -1891,7 +1887,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="2"/>
@@ -1908,46 +1904,46 @@
         <v xml:space="preserve">**Over-age lower secondary students.** </v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+    <row r="47" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C47" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F47" s="7" t="str">
+      <c r="B47" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C47" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="5" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Qualified teachers in primary education.** </v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="7" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:6" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F48" s="7" t="str">
+      <c r="B48" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C48" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F48" s="5" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Qualified teachers in secondary education.** </v>
       </c>
@@ -1957,7 +1953,7 @@
         <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="2"/>
@@ -1979,7 +1975,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="2"/>
@@ -2001,7 +1997,7 @@
         <v>13</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="2"/>
@@ -2023,7 +2019,7 @@
         <v>42</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="2"/>
@@ -2045,7 +2041,7 @@
         <v>43</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="2"/>
@@ -2067,7 +2063,7 @@
         <v>44</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="2"/>
@@ -2089,7 +2085,7 @@
         <v>4</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="2"/>
@@ -2111,7 +2107,7 @@
         <v>79</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="2"/>
@@ -2133,7 +2129,7 @@
         <v>5</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="2"/>
@@ -2155,7 +2151,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="2"/>
@@ -2177,7 +2173,7 @@
         <v>60</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="2"/>
@@ -2199,7 +2195,7 @@
         <v>82</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="2"/>
@@ -2221,7 +2217,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="2"/>
@@ -2243,7 +2239,7 @@
         <v>84</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="2"/>
@@ -2265,7 +2261,7 @@
         <v>83</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="2"/>
@@ -2287,7 +2283,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="2"/>
@@ -2309,7 +2305,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="2"/>
@@ -2326,24 +2322,24 @@
         <v xml:space="preserve">**Youth literacy rate.** </v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
+    <row r="66" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C66" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>%</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E66" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F66" s="7" t="str">
+      <c r="B66" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C66" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F66" s="5" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">**Satisfied demand for family planning.** </v>
       </c>
@@ -2353,7 +2349,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C79" si="3">IF(D67="%","%","")</f>
@@ -2370,21 +2366,21 @@
         <v xml:space="preserve">**HPV vaccination rate, last dose.** </v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>80</v>
       </c>
-      <c r="B68" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C68" s="5" t="str">
+      <c r="B68" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C68" t="str">
         <f t="shared" si="3"/>
         <v>%</v>
       </c>
-      <c r="D68" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F68" s="5" t="str">
+      <c r="D68" t="s">
+        <v>54</v>
+      </c>
+      <c r="F68" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">**High skill employment rate.** </v>
       </c>
@@ -2394,7 +2390,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="3"/>
@@ -2416,7 +2412,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="3"/>
@@ -2438,7 +2434,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="3"/>
@@ -2460,7 +2456,7 @@
         <v>72</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="3"/>
@@ -2482,7 +2478,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="3"/>
@@ -2504,7 +2500,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="3"/>
@@ -2523,7 +2519,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="3"/>
@@ -2542,7 +2538,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="3"/>
@@ -2561,7 +2557,7 @@
         <v>77</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="3"/>
@@ -2580,7 +2576,7 @@
         <v>78</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="3"/>
@@ -2594,12 +2590,12 @@
         <v xml:space="preserve">**Internally Displaced Persons.** </v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>81</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Add SDG and UNESCO and update clean
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -916,8 +916,8 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modify PDF and solve brief texts
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{0E1B8E99-ACE7-4DD0-B566-889CEC5B3EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E422A5D-362E-4DF2-A4AA-97FB28E22649}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0E1B8E99-ACE7-4DD0-B566-889CEC5B3EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18AD5ECE-A299-4016-817E-B505B3843A11}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -362,9 +362,6 @@
     <t>**Prevalence of insufficient physical activity.** The share of school-going adolescents (ages 11-17) not meeting WHO recommendations on physical activity for health is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Children who are developmentally on track.** In `ind_year', **`ind_value'%** of children (ages 24-59 months) were developmentally on track in health, learning and psychosocial well-being</t>
-  </si>
-  <si>
     <t>**HIV incidence rate.** The estimated number of new HIV infections per 1,000 uninfected adolescents (ages 10-19 years) is **`ind_value'** (`ind_year')</t>
   </si>
   <si>
@@ -485,9 +482,6 @@
     <t>**Care seeking for febrile children.** In `ind_year', **`ind_value'%** of children under age 5 with a fever for whom medical advice or treatment was sought</t>
   </si>
   <si>
-    <t>**Minimum meal frequency.** The share of children ages 0-23 months who regularly consume an age-appropriate meal is **`ind_value'%** (`ind_year')</t>
-  </si>
-  <si>
     <t>**High skill employment rate.** In `ind_year', **`ind_value'%** of employed adults worked in high-skilled occupations</t>
   </si>
   <si>
@@ -537,6 +531,12 @@
   </si>
   <si>
     <t>**DTP vaccination rate, third dose.** In `ind_year', **`ind_value'%** of infants received the third dose of the diphtheria, tetanus and pertussis vaccine</t>
+  </si>
+  <si>
+    <t>**Minimum meal frequency.** The share of children ages 6-23 months who regularly consume an age-appropriate meal is **`ind_value'%** (`ind_year')</t>
+  </si>
+  <si>
+    <t>**Children who are developmentally on track.** In `ind_year', **`ind_value'%** of children (ages 36-59 months) were developmentally on track in health, learning and psychosocial well-being</t>
   </si>
 </sst>
 </file>
@@ -916,8 +916,8 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +954,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
         <v>69</v>
@@ -972,7 +972,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C34" si="0">IF(D3="%","%","")</f>
@@ -994,7 +994,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -1060,7 +1060,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -1126,7 +1126,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -1148,7 +1148,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -1192,7 +1192,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -1214,7 +1214,7 @@
         <v>85</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -1236,7 +1236,7 @@
         <v>86</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -1258,7 +1258,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -1280,7 +1280,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -1302,7 +1302,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -1368,7 +1368,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -1387,7 +1387,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -1428,7 +1428,7 @@
         <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -1450,7 +1450,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -1472,7 +1472,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -1494,7 +1494,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -1513,7 +1513,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -1551,7 +1551,7 @@
         <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -1595,7 +1595,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -1617,7 +1617,7 @@
         <v>25</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -1639,7 +1639,7 @@
         <v>38</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -1702,7 +1702,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="2"/>
@@ -1721,7 +1721,7 @@
         <v>52</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="2"/>
@@ -1743,7 +1743,7 @@
         <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="2"/>
@@ -1765,7 +1765,7 @@
         <v>33</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C40" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1787,7 +1787,7 @@
         <v>30</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C41" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1809,7 +1809,7 @@
         <v>14</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C42" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1831,7 +1831,7 @@
         <v>15</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C43" s="7" t="str">
         <f t="shared" si="2"/>
@@ -1853,7 +1853,7 @@
         <v>34</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C44" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1875,7 +1875,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="2"/>
@@ -1897,7 +1897,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="2"/>
@@ -1919,7 +1919,7 @@
         <v>19</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="2"/>
@@ -1941,7 +1941,7 @@
         <v>20</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="2"/>
@@ -1963,7 +1963,7 @@
         <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="2"/>
@@ -1985,7 +1985,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="2"/>
@@ -2007,7 +2007,7 @@
         <v>13</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="2"/>
@@ -2029,7 +2029,7 @@
         <v>42</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="2"/>
@@ -2051,7 +2051,7 @@
         <v>43</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="2"/>
@@ -2073,7 +2073,7 @@
         <v>44</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="2"/>
@@ -2095,7 +2095,7 @@
         <v>4</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="2"/>
@@ -2117,7 +2117,7 @@
         <v>79</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="2"/>
@@ -2139,7 +2139,7 @@
         <v>5</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="2"/>
@@ -2161,7 +2161,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>107</v>
+        <v>165</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="2"/>
@@ -2183,7 +2183,7 @@
         <v>60</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="2"/>
@@ -2249,7 +2249,7 @@
         <v>84</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="2"/>
@@ -2271,7 +2271,7 @@
         <v>83</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="2"/>
@@ -2293,7 +2293,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="2"/>
@@ -2315,7 +2315,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="2"/>
@@ -2337,7 +2337,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="2"/>
@@ -2359,7 +2359,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C79" si="3">IF(D67="%","%","")</f>
@@ -2381,7 +2381,7 @@
         <v>80</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="3"/>
@@ -2422,7 +2422,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="3"/>
@@ -2444,7 +2444,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="3"/>
@@ -2488,7 +2488,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="3"/>
@@ -2510,7 +2510,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="3"/>
@@ -2529,7 +2529,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="3"/>
@@ -2605,7 +2605,7 @@
         <v>81</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C79" s="5" t="str">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Update: suicide rates + UIS SDGs
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/briefs_texts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0E1B8E99-ACE7-4DD0-B566-889CEC5B3EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18AD5ECE-A299-4016-817E-B505B3843A11}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{0E1B8E99-ACE7-4DD0-B566-889CEC5B3EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03FB0507-E369-4F22-AFCA-969BFC4C1E95}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$79</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -398,9 +398,6 @@
     <t>**Adolescent fertility rate.** The number of births for every 1,000 women ages 15-19 is **`ind_value'** (`ind_year')</t>
   </si>
   <si>
-    <t>**Gross enrollment in early childhood education.** In `ind_year',  **`ind_value'%**  of children were enrolled at early childhood education</t>
-  </si>
-  <si>
     <t>**Child mortality rate.**  The mortality rate for children ages 5-14 is **`ind_value'** per 1,000 children aged 5 (`ind_year')</t>
   </si>
   <si>
@@ -512,9 +509,6 @@
     <t>**Care seeking for children with diarrhea.** The share of children (ages 0-5) with diarrhea who attended a health facility is  **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
-    <t>**Gross enrollment rate, early childhood education.** In `ind_year', **`ind_value'%** of children at the official age for the corresponding level were enrolled in an early childhood educational development program</t>
-  </si>
-  <si>
     <t>**Upper secondary school completion rate.** The upper-secondary completion rate at ages 3-5 years above the intended age for the last grade of that level is **`ind_value'%** (`ind_year')</t>
   </si>
   <si>
@@ -537,6 +531,12 @@
   </si>
   <si>
     <t>**Children who are developmentally on track.** In `ind_year', **`ind_value'%** of children (ages 36-59 months) were developmentally on track in health, learning and psychosocial well-being</t>
+  </si>
+  <si>
+    <t>**Gross enrollment in early childhood education.** In `ind_year',  **`ind_value'%**  of children were enrolled in an early childhood educational development program</t>
+  </si>
+  <si>
+    <t>**Gross enrollment rate, early childhood education.** In `ind_year', **`ind_value'%** of children at the official age for the corresponding level were enrolled at early childhood education</t>
   </si>
 </sst>
 </file>
@@ -648,6 +648,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -916,8 +920,8 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,7 +998,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -1060,7 +1064,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -1126,7 +1130,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -1148,7 +1152,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -1192,7 +1196,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -1214,7 +1218,7 @@
         <v>85</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -1236,7 +1240,7 @@
         <v>86</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -1280,7 +1284,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -1302,7 +1306,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -1387,7 +1391,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -1450,7 +1454,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -1472,7 +1476,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -1494,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -1513,7 +1517,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -1551,7 +1555,7 @@
         <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -1595,7 +1599,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -1617,7 +1621,7 @@
         <v>25</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -1639,7 +1643,7 @@
         <v>38</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -1702,7 +1706,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="2"/>
@@ -1721,7 +1725,7 @@
         <v>52</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="2"/>
@@ -1743,7 +1747,7 @@
         <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="2"/>
@@ -1765,7 +1769,7 @@
         <v>33</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C40" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1787,7 +1791,7 @@
         <v>30</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C41" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1809,7 +1813,7 @@
         <v>14</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C42" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1826,12 +1830,12 @@
         <v xml:space="preserve">**Upper secondary school completion rate.** </v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="C43" s="7" t="str">
         <f t="shared" si="2"/>
@@ -1853,7 +1857,7 @@
         <v>34</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C44" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1875,7 +1879,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="2"/>
@@ -1897,7 +1901,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="2"/>
@@ -1919,7 +1923,7 @@
         <v>19</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="2"/>
@@ -1941,7 +1945,7 @@
         <v>20</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="2"/>
@@ -1963,7 +1967,7 @@
         <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="2"/>
@@ -1985,7 +1989,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="2"/>
@@ -2007,7 +2011,7 @@
         <v>13</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="2"/>
@@ -2029,7 +2033,7 @@
         <v>42</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="2"/>
@@ -2051,7 +2055,7 @@
         <v>43</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="2"/>
@@ -2073,7 +2077,7 @@
         <v>44</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="2"/>
@@ -2117,7 +2121,7 @@
         <v>79</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="2"/>
@@ -2161,7 +2165,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="2"/>
@@ -2183,7 +2187,7 @@
         <v>60</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="2"/>
@@ -2249,7 +2253,7 @@
         <v>84</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="2"/>
@@ -2271,7 +2275,7 @@
         <v>83</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="2"/>
@@ -2315,7 +2319,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="2"/>
@@ -2337,7 +2341,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="2"/>
@@ -2381,7 +2385,7 @@
         <v>80</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="3"/>
@@ -2488,7 +2492,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="3"/>
@@ -2510,7 +2514,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="3"/>
@@ -2605,7 +2609,7 @@
         <v>81</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C79" s="5" t="str">
         <f t="shared" si="3"/>
@@ -2620,7 +2624,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E73" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E79" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataValidations count="1">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A76:A78 A74 A2:A57" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>

</xml_diff>